<commit_message>
Updated Excel barriers, still to work on missing species
</commit_message>
<xml_diff>
--- a/Windows/Busquedas/Barriers/Orthoptera/Orthoptera_Barriers.xlsx
+++ b/Windows/Busquedas/Barriers/Orthoptera/Orthoptera_Barriers.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\Documents\GitHub\Interespecific_hybrids\Windows\Busquedas\Barriers\Orthoptera\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Barriers" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Info" sheetId="1" r:id="rId1"/>
+    <sheet name="Barriers" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Barriers!$A$1:$H$439</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1">Barriers!$A$1:$H$439</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -27,320 +31,317 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="102">
   <si>
-    <t xml:space="preserve">Barrier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Choice-Mating</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A choice mating is considered either when choice matings experiments are done and heterospecific crosses develop or when hybridisation is known to happen in nature, e. g. hybrid zone development</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hybrid-Egg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mating results in hybrid egg production</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hybrid-Adult</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hybrid eggs survive and develop into adults</t>
-  </si>
-  <si>
-    <t xml:space="preserve">One-Sex-Fertile-Hybrids</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Only one of the hybrid sex is fertile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fertile-Hybrids</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It is reported both hybrid sexes to be fertile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOTE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If in any part of the article, it is reported the esxistance of natural hybrids or hybrid zones, barriers are automatically assumed to allow gene flow until the formation of adult hybrids</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOTE2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revised articles were read in detail looking for the level of isolation between species-pairs. Even if barriers were described in the introduction / methods and cited from another paper data was recorded</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sp1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sp2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Condition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Authors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Article</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Author-Year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Article2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Orchelimum nigripes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Orchelimum pulchellum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Laboratory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shapiro, LH.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reproductive costs to heterospecific mating between two hybridizing katydids (Orthoptera : Tettigoniidae)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chorthippus brunneus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chorthippus jacobsi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saldamando, CI; Tatsuta, H; Butlin, RK.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hybrids between Chorthippus brunneus and C-jacobsi (Orthoptera : Acrididae) do not show endogenous postzygotic isolation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tetrix undulata</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tetrix subulata</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hochkirch, A; Bucker, A; Groning, J</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reproductive Interference between the Common Ground-hopper Tetrix undulata and the Slender Ground-hopper Tetrix subulata (Orthoptera, Tetrigidae)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allonemobius fasciatus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allonemobius socius</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GREGORY, PG; HOWARD, DJ.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LABORATORY HYBRIDIZATION STUDIES OF ALLONEMOBIUS-FASCIATUS AND A-SOCIUS (ORTHOPTERA, GRYLLIDAE)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cyphoderris buckelli</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cyphoderris monstrosa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Field</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dupuis, JR; Judge, KA; Brunet, BMT; Chan, SO; Sperling, FAH.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Does hunger lead to hybridization in a genus of sexually cannibalistic insects (Orthoptera: Prophalangopsidae)?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chorthippus albomarginatus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chorthippus oschei</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vedenina, VY; Kulygina, NK; Panyutin, AK.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Isolation mechanisms in the closely related grasshopper species, Chorthippus albomarginatus and Ch. oschei (Orthoptera, Acrididae)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chorthippus biguttulus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gottsberger, B; Mayer, F.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dominance effects strengthen premating hybridization barriers between sympatric species of grasshoppers (Acrididae, Orthoptera)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hybrid males are behavioraly infertile because songs fail to attract females</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gottsberger, B; Mayer, F. 2007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Behavioral sterility of hybrid males in acoustically communicating grasshoppers (Acrididae, Gomphocerinae)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chorthippus karelini</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vedenina, VY.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COURTSHIP SONG ANALYSIS IN TWO HYBRID ZONES BETWEEN SIBLING SPECIES OF THE CHORTHIPPUS ALBOMARGINATUS GROUP (ORTHOPTERA, GOMPHOCERINAE)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dociostaurus curvicercus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dociostaurus jagoi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BLONDHEIM, SA.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PATTERNS OF REPRODUCTIVE ISOLATION BETWEEN THE SIBLING GRASSHOPPER SPECIES DOCIOSTAURUS-CURVICERCUS AND D-JAGOI-JAGOI (ORTHOPTERA, ACRIDIDAE, GOMPHOCERINAE)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Podisma tyatiensis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Podisma sapporensis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bugrov, AG; Warchalowska-Sliwa, E; Akimoto, S.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taxonomic status of the grasshopper Podisma tyatiensis and reproductive isolation between P-tyatiensis and Podisma sapporensis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tetrix ceperoi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hochkirch, A; Deppermann, J; Groning, J.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Visual communication behaviour as a mechanism behind reproductive interference in three pygmy grasshoppers (Genus Tetrix, tetrigidae, orthoptera)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chorthippus mollis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finck, J; Ronacher, B.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Components of reproductive isolation between the closely related grasshopper species Chorthippus biguttulus and C. mollis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gryllus staccato</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gryllus lineaticeps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gray, DA; Gutierrez, NJ; Chen, TL; Gonzalez, C; Weissman, DB; Cole, JA.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Species divergence in field crickets: genetics, song, ecomorphology, and pre- and postzygotic isolation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gryllus personatus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gryllus bimaculatus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gryllus campestris</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Veen, T; Faulks, J; Tyler, F; Lloyd, J; Tregenza, T.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diverse reproductive barriers in hybridising crickets suggests extensive variation in the evolution and maintenance of isolation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Melanoplus sanguinipes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Melanoplus devastator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Orr, MR.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Life-history adaptation and reproductive isolation in a grasshopper hybrid zone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gryllus firmus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gryllus pennsylvanicus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maroja, LS; Andres, JA; Walters, JR; Harrison, RG.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multiple barriers to gene exchange in a field cricket hybrid zone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chorthippus parallelus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chorthippus montanus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rohde, K; Hau, Y; Weyer, J; Hochkirch, A.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wide prevalence of hybridization in two sympatric grasshopper species may be shaped by their relative abundances</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stenobothrus rubicundus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stenobothrus clavatus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sradnick, J; Klopfel, A; Elsner, N; Vedenina, V.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Variation in complex mating signals in an "island" hybrid zone between Stenobothrus grasshopper species</t>
+    <t>Barrier</t>
+  </si>
+  <si>
+    <t>Information</t>
+  </si>
+  <si>
+    <t>Choice-Mating</t>
+  </si>
+  <si>
+    <t>A choice mating is considered either when choice matings experiments are done and heterospecific crosses develop or when hybridisation is known to happen in nature, e. g. hybrid zone development</t>
+  </si>
+  <si>
+    <t>Hybrid-Egg</t>
+  </si>
+  <si>
+    <t>Mating results in hybrid egg production</t>
+  </si>
+  <si>
+    <t>Hybrid-Adult</t>
+  </si>
+  <si>
+    <t>Hybrid eggs survive and develop into adults</t>
+  </si>
+  <si>
+    <t>One-Sex-Fertile-Hybrids</t>
+  </si>
+  <si>
+    <t>Only one of the hybrid sex is fertile</t>
+  </si>
+  <si>
+    <t>Fertile-Hybrids</t>
+  </si>
+  <si>
+    <t>It is reported both hybrid sexes to be fertile</t>
+  </si>
+  <si>
+    <t>NOTE</t>
+  </si>
+  <si>
+    <t>If in any part of the article, it is reported the esxistance of natural hybrids or hybrid zones, barriers are automatically assumed to allow gene flow until the formation of adult hybrids</t>
+  </si>
+  <si>
+    <t>NOTE2</t>
+  </si>
+  <si>
+    <t>Revised articles were read in detail looking for the level of isolation between species-pairs. Even if barriers were described in the introduction / methods and cited from another paper data was recorded</t>
+  </si>
+  <si>
+    <t>Sp1</t>
+  </si>
+  <si>
+    <t>Sp2</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Authors</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Article</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Author-Year</t>
+  </si>
+  <si>
+    <t>Article2</t>
+  </si>
+  <si>
+    <t>Orchelimum nigripes</t>
+  </si>
+  <si>
+    <t>Orchelimum pulchellum</t>
+  </si>
+  <si>
+    <t>Laboratory</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Shapiro, LH.</t>
+  </si>
+  <si>
+    <t>Reproductive costs to heterospecific mating between two hybridizing katydids (Orthoptera : Tettigoniidae)</t>
+  </si>
+  <si>
+    <t>Chorthippus brunneus</t>
+  </si>
+  <si>
+    <t>Chorthippus jacobsi</t>
+  </si>
+  <si>
+    <t>Saldamando, CI; Tatsuta, H; Butlin, RK.</t>
+  </si>
+  <si>
+    <t>Hybrids between Chorthippus brunneus and C-jacobsi (Orthoptera : Acrididae) do not show endogenous postzygotic isolation</t>
+  </si>
+  <si>
+    <t>Tetrix undulata</t>
+  </si>
+  <si>
+    <t>Tetrix subulata</t>
+  </si>
+  <si>
+    <t>Hochkirch, A; Bucker, A; Groning, J</t>
+  </si>
+  <si>
+    <t>Reproductive Interference between the Common Ground-hopper Tetrix undulata and the Slender Ground-hopper Tetrix subulata (Orthoptera, Tetrigidae)</t>
+  </si>
+  <si>
+    <t>Allonemobius fasciatus</t>
+  </si>
+  <si>
+    <t>Allonemobius socius</t>
+  </si>
+  <si>
+    <t>GREGORY, PG; HOWARD, DJ.</t>
+  </si>
+  <si>
+    <t>LABORATORY HYBRIDIZATION STUDIES OF ALLONEMOBIUS-FASCIATUS AND A-SOCIUS (ORTHOPTERA, GRYLLIDAE)</t>
+  </si>
+  <si>
+    <t>Cyphoderris buckelli</t>
+  </si>
+  <si>
+    <t>Cyphoderris monstrosa</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Dupuis, JR; Judge, KA; Brunet, BMT; Chan, SO; Sperling, FAH.</t>
+  </si>
+  <si>
+    <t>Does hunger lead to hybridization in a genus of sexually cannibalistic insects (Orthoptera: Prophalangopsidae)?</t>
+  </si>
+  <si>
+    <t>Chorthippus albomarginatus</t>
+  </si>
+  <si>
+    <t>Chorthippus oschei</t>
+  </si>
+  <si>
+    <t>Vedenina, VY; Kulygina, NK; Panyutin, AK.</t>
+  </si>
+  <si>
+    <t>Isolation mechanisms in the closely related grasshopper species, Chorthippus albomarginatus and Ch. oschei (Orthoptera, Acrididae)</t>
+  </si>
+  <si>
+    <t>Chorthippus biguttulus</t>
+  </si>
+  <si>
+    <t>Gottsberger, B; Mayer, F.</t>
+  </si>
+  <si>
+    <t>Dominance effects strengthen premating hybridization barriers between sympatric species of grasshoppers (Acrididae, Orthoptera)</t>
+  </si>
+  <si>
+    <t>Hybrid males are behavioraly infertile because songs fail to attract females</t>
+  </si>
+  <si>
+    <t>Gottsberger, B; Mayer, F. 2007</t>
+  </si>
+  <si>
+    <t>Behavioral sterility of hybrid males in acoustically communicating grasshoppers (Acrididae, Gomphocerinae)</t>
+  </si>
+  <si>
+    <t>Chorthippus karelini</t>
+  </si>
+  <si>
+    <t>Vedenina, VY.</t>
+  </si>
+  <si>
+    <t>COURTSHIP SONG ANALYSIS IN TWO HYBRID ZONES BETWEEN SIBLING SPECIES OF THE CHORTHIPPUS ALBOMARGINATUS GROUP (ORTHOPTERA, GOMPHOCERINAE)</t>
+  </si>
+  <si>
+    <t>Dociostaurus curvicercus</t>
+  </si>
+  <si>
+    <t>Dociostaurus jagoi</t>
+  </si>
+  <si>
+    <t>BLONDHEIM, SA.</t>
+  </si>
+  <si>
+    <t>PATTERNS OF REPRODUCTIVE ISOLATION BETWEEN THE SIBLING GRASSHOPPER SPECIES DOCIOSTAURUS-CURVICERCUS AND D-JAGOI-JAGOI (ORTHOPTERA, ACRIDIDAE, GOMPHOCERINAE)</t>
+  </si>
+  <si>
+    <t>Podisma tyatiensis</t>
+  </si>
+  <si>
+    <t>Podisma sapporensis</t>
+  </si>
+  <si>
+    <t>Bugrov, AG; Warchalowska-Sliwa, E; Akimoto, S.</t>
+  </si>
+  <si>
+    <t>Taxonomic status of the grasshopper Podisma tyatiensis and reproductive isolation between P-tyatiensis and Podisma sapporensis</t>
+  </si>
+  <si>
+    <t>Tetrix ceperoi</t>
+  </si>
+  <si>
+    <t>Hochkirch, A; Deppermann, J; Groning, J.</t>
+  </si>
+  <si>
+    <t>Visual communication behaviour as a mechanism behind reproductive interference in three pygmy grasshoppers (Genus Tetrix, tetrigidae, orthoptera)</t>
+  </si>
+  <si>
+    <t>Chorthippus mollis</t>
+  </si>
+  <si>
+    <t>Finck, J; Ronacher, B.</t>
+  </si>
+  <si>
+    <t>Components of reproductive isolation between the closely related grasshopper species Chorthippus biguttulus and C. mollis</t>
+  </si>
+  <si>
+    <t>Gryllus staccato</t>
+  </si>
+  <si>
+    <t>Gryllus lineaticeps</t>
+  </si>
+  <si>
+    <t>Gray, DA; Gutierrez, NJ; Chen, TL; Gonzalez, C; Weissman, DB; Cole, JA.</t>
+  </si>
+  <si>
+    <t>Species divergence in field crickets: genetics, song, ecomorphology, and pre- and postzygotic isolation</t>
+  </si>
+  <si>
+    <t>Gryllus personatus</t>
+  </si>
+  <si>
+    <t>Gryllus bimaculatus</t>
+  </si>
+  <si>
+    <t>Gryllus campestris</t>
+  </si>
+  <si>
+    <t>Veen, T; Faulks, J; Tyler, F; Lloyd, J; Tregenza, T.</t>
+  </si>
+  <si>
+    <t>Diverse reproductive barriers in hybridising crickets suggests extensive variation in the evolution and maintenance of isolation</t>
+  </si>
+  <si>
+    <t>Melanoplus sanguinipes</t>
+  </si>
+  <si>
+    <t>Melanoplus devastator</t>
+  </si>
+  <si>
+    <t>Orr, MR.</t>
+  </si>
+  <si>
+    <t>Life-history adaptation and reproductive isolation in a grasshopper hybrid zone</t>
+  </si>
+  <si>
+    <t>Gryllus firmus</t>
+  </si>
+  <si>
+    <t>Gryllus pennsylvanicus</t>
+  </si>
+  <si>
+    <t>Maroja, LS; Andres, JA; Walters, JR; Harrison, RG.</t>
+  </si>
+  <si>
+    <t>Multiple barriers to gene exchange in a field cricket hybrid zone</t>
+  </si>
+  <si>
+    <t>Chorthippus parallelus</t>
+  </si>
+  <si>
+    <t>Chorthippus montanus</t>
+  </si>
+  <si>
+    <t>Rohde, K; Hau, Y; Weyer, J; Hochkirch, A.</t>
+  </si>
+  <si>
+    <t>Wide prevalence of hybridization in two sympatric grasshopper species may be shaped by their relative abundances</t>
+  </si>
+  <si>
+    <t>Stenobothrus rubicundus</t>
+  </si>
+  <si>
+    <t>Stenobothrus clavatus</t>
+  </si>
+  <si>
+    <t>Sradnick, J; Klopfel, A; Elsner, N; Vedenina, V.</t>
+  </si>
+  <si>
+    <t>Variation in complex mating signals in an "island" hybrid zone between Stenobothrus grasshopper species</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -349,22 +350,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -381,7 +367,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -389,82 +375,314 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="A1:H22"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="A1:H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.57"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -472,98 +690,90 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:H22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="22.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="167.85"/>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="167.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -607,14 +817,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>27</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -632,24 +842,24 @@
       <c r="H2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="J2">
         <v>2000</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="K2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>27</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -667,24 +877,24 @@
       <c r="H3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="0" t="n">
+      <c r="J3">
         <v>2005</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="K3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -702,24 +912,24 @@
       <c r="H4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="I4" t="s">
         <v>38</v>
       </c>
-      <c r="J4" s="0" t="n">
+      <c r="J4">
         <v>2008</v>
       </c>
-      <c r="K4" s="0" t="s">
+      <c r="K4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>27</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -737,24 +947,24 @@
       <c r="H5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="I5" t="s">
         <v>42</v>
       </c>
-      <c r="J5" s="0" t="n">
+      <c r="J5">
         <v>1993</v>
       </c>
-      <c r="K5" s="0" t="s">
+      <c r="K5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>46</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -772,24 +982,24 @@
       <c r="H6" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="I6" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="0" t="n">
+      <c r="J6">
         <v>2020</v>
       </c>
-      <c r="K6" s="0" t="s">
+      <c r="K6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -807,24 +1017,24 @@
       <c r="H7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="I7" t="s">
         <v>52</v>
       </c>
-      <c r="J7" s="0" t="n">
+      <c r="J7">
         <v>2007</v>
       </c>
-      <c r="K7" s="0" t="s">
+      <c r="K7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" t="s">
         <v>27</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -842,33 +1052,33 @@
       <c r="H8" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="I8" s="0" t="s">
+      <c r="I8" t="s">
         <v>55</v>
       </c>
-      <c r="J8" s="0" t="n">
+      <c r="J8">
         <v>2019</v>
       </c>
-      <c r="K8" s="0" t="s">
+      <c r="K8" t="s">
         <v>56</v>
       </c>
-      <c r="L8" s="0" t="s">
+      <c r="L8" t="s">
         <v>57</v>
       </c>
-      <c r="M8" s="0" t="s">
+      <c r="M8" t="s">
         <v>58</v>
       </c>
-      <c r="N8" s="0" t="s">
+      <c r="N8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" t="s">
         <v>27</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -886,24 +1096,24 @@
       <c r="H9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I9" s="0" t="s">
+      <c r="I9" t="s">
         <v>61</v>
       </c>
-      <c r="J9" s="0" t="n">
+      <c r="J9">
         <v>2015</v>
       </c>
-      <c r="K9" s="0" t="s">
+      <c r="K9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -921,24 +1131,24 @@
       <c r="H10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="0" t="s">
+      <c r="I10" t="s">
         <v>61</v>
       </c>
-      <c r="J10" s="0" t="n">
+      <c r="J10">
         <v>2015</v>
       </c>
-      <c r="K10" s="0" t="s">
+      <c r="K10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -956,24 +1166,24 @@
       <c r="H11" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="I11" s="0" t="s">
+      <c r="I11" t="s">
         <v>65</v>
       </c>
-      <c r="J11" s="0" t="n">
+      <c r="J11">
         <v>1990</v>
       </c>
-      <c r="K11" s="0" t="s">
+      <c r="K11" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>67</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" t="s">
         <v>68</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="3" t="s">
@@ -991,24 +1201,24 @@
       <c r="H12" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="I12" s="0" t="s">
+      <c r="I12" t="s">
         <v>69</v>
       </c>
-      <c r="J12" s="0" t="n">
+      <c r="J12">
         <v>2005</v>
       </c>
-      <c r="K12" s="0" t="s">
+      <c r="K12" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" t="s">
         <v>46</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -1026,28 +1236,28 @@
       <c r="H13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I13" s="0" t="s">
+      <c r="I13" t="s">
         <v>72</v>
       </c>
-      <c r="J13" s="0" t="n">
+      <c r="J13">
         <v>2006</v>
       </c>
-      <c r="K13" s="0" t="s">
+      <c r="K13" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" t="s">
         <v>27</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>28</v>
@@ -1061,24 +1271,24 @@
       <c r="H14" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="I14" s="0" t="s">
+      <c r="I14" t="s">
         <v>75</v>
       </c>
-      <c r="J14" s="0" t="n">
+      <c r="J14">
         <v>2017</v>
       </c>
-      <c r="K14" s="0" t="s">
+      <c r="K14" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>77</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" t="s">
         <v>78</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="3" t="s">
@@ -1096,24 +1306,24 @@
       <c r="H15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I15" s="0" t="s">
+      <c r="I15" t="s">
         <v>79</v>
       </c>
-      <c r="J15" s="0" t="n">
+      <c r="J15">
         <v>2016</v>
       </c>
-      <c r="K15" s="0" t="s">
+      <c r="K15" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>77</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="3" t="s">
@@ -1131,24 +1341,24 @@
       <c r="H16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="0" t="s">
+      <c r="I16" t="s">
         <v>79</v>
       </c>
-      <c r="J16" s="0" t="n">
+      <c r="J16">
         <v>2016</v>
       </c>
-      <c r="K16" s="0" t="s">
+      <c r="K16" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" t="s">
         <v>81</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" t="s">
         <v>27</v>
       </c>
       <c r="D17" s="3" t="s">
@@ -1166,24 +1376,24 @@
       <c r="H17" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I17" s="0" t="s">
+      <c r="I17" t="s">
         <v>79</v>
       </c>
-      <c r="J17" s="0" t="n">
+      <c r="J17">
         <v>2016</v>
       </c>
-      <c r="K17" s="0" t="s">
+      <c r="K17" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>82</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" t="s">
         <v>83</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" t="s">
         <v>27</v>
       </c>
       <c r="D18" s="3" t="s">
@@ -1201,24 +1411,24 @@
       <c r="H18" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I18" s="0" t="s">
+      <c r="I18" t="s">
         <v>84</v>
       </c>
-      <c r="J18" s="0" t="n">
+      <c r="J18">
         <v>2013</v>
       </c>
-      <c r="K18" s="0" t="s">
+      <c r="K18" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>86</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" t="s">
         <v>27</v>
       </c>
       <c r="D19" s="3" t="s">
@@ -1236,24 +1446,24 @@
       <c r="H19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I19" s="0" t="s">
+      <c r="I19" t="s">
         <v>88</v>
       </c>
-      <c r="J19" s="0" t="n">
+      <c r="J19">
         <v>1996</v>
       </c>
-      <c r="K19" s="0" t="s">
+      <c r="K19" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>90</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" t="s">
         <v>91</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" t="s">
         <v>27</v>
       </c>
       <c r="D20" s="3" t="s">
@@ -1271,24 +1481,24 @@
       <c r="H20" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I20" s="0" t="s">
+      <c r="I20" t="s">
         <v>92</v>
       </c>
-      <c r="J20" s="0" t="n">
+      <c r="J20">
         <v>2009</v>
       </c>
-      <c r="K20" s="0" t="s">
+      <c r="K20" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>94</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" t="s">
         <v>95</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" t="s">
         <v>27</v>
       </c>
       <c r="D21" s="3" t="s">
@@ -1306,24 +1516,24 @@
       <c r="H21" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I21" s="0" t="s">
+      <c r="I21" t="s">
         <v>96</v>
       </c>
-      <c r="J21" s="0" t="n">
+      <c r="J21">
         <v>2015</v>
       </c>
-      <c r="K21" s="0" t="s">
+      <c r="K21" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>98</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" t="s">
         <v>99</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" t="s">
         <v>27</v>
       </c>
       <c r="D22" s="3" t="s">
@@ -1341,17 +1551,17 @@
       <c r="H22" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I22" s="0" t="s">
+      <c r="I22" t="s">
         <v>100</v>
       </c>
-      <c r="J22" s="0" t="n">
+      <c r="J22">
         <v>2016</v>
       </c>
-      <c r="K22" s="0" t="s">
+      <c r="K22" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F39" s="3" t="s">
         <v>28</v>
       </c>
@@ -1359,7 +1569,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F40" s="3" t="s">
         <v>28</v>
       </c>
@@ -1367,7 +1577,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F41" s="3" t="s">
         <v>28</v>
       </c>
@@ -1376,30 +1586,22 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:H22"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -1425,14 +1627,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>27</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -1451,14 +1653,14 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>27</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -1477,14 +1679,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -1503,14 +1705,14 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>27</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -1529,14 +1731,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>46</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -1555,14 +1757,14 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -1581,14 +1783,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" t="s">
         <v>27</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -1607,14 +1809,14 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" t="s">
         <v>27</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -1633,14 +1835,14 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -1659,14 +1861,14 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -1685,14 +1887,14 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>67</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" t="s">
         <v>68</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="3" t="s">
@@ -1711,14 +1913,14 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" t="s">
         <v>46</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -1737,14 +1939,14 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" t="s">
         <v>27</v>
       </c>
       <c r="D14" s="3" t="s">
@@ -1763,14 +1965,14 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>77</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" t="s">
         <v>78</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="3" t="s">
@@ -1789,14 +1991,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>77</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="3" t="s">
@@ -1815,14 +2017,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" t="s">
         <v>81</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" t="s">
         <v>27</v>
       </c>
       <c r="D17" s="3" t="s">
@@ -1841,14 +2043,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>82</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" t="s">
         <v>83</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" t="s">
         <v>27</v>
       </c>
       <c r="D18" s="3" t="s">
@@ -1867,14 +2069,14 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>86</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" t="s">
         <v>27</v>
       </c>
       <c r="D19" s="3" t="s">
@@ -1893,14 +2095,14 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>90</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" t="s">
         <v>91</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" t="s">
         <v>27</v>
       </c>
       <c r="D20" s="3" t="s">
@@ -1919,14 +2121,14 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>94</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" t="s">
         <v>95</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" t="s">
         <v>27</v>
       </c>
       <c r="D21" s="3" t="s">
@@ -1945,14 +2147,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>98</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" t="s">
         <v>99</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" t="s">
         <v>27</v>
       </c>
       <c r="D22" s="3" t="s">
@@ -1972,10 +2174,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>